<commit_message>
added hopes and risks as variable
</commit_message>
<xml_diff>
--- a/ML_PL_new/modinput_odds_tx.xlsx
+++ b/ML_PL_new/modinput_odds_tx.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q299"/>
+  <dimension ref="A1:Q329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15626,6 +15626,1476 @@
       <c r="P299" t="inlineStr"/>
       <c r="Q299" t="inlineStr"/>
     </row>
+    <row r="300">
+      <c r="A300" s="2" t="n">
+        <v>45800.79166666666</v>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t>Betis</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="D300" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E300" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="F300" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="G300" t="n">
+        <v>3.45</v>
+      </c>
+      <c r="H300" t="inlineStr"/>
+      <c r="I300" t="inlineStr"/>
+      <c r="J300" t="inlineStr"/>
+      <c r="K300" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="L300" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M300" t="n">
+        <v>1.26</v>
+      </c>
+      <c r="N300" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="O300" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="P300" t="inlineStr"/>
+      <c r="Q300" t="inlineStr"/>
+    </row>
+    <row r="301">
+      <c r="A301" s="2" t="n">
+        <v>45800.86458333334</v>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t>Como</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>Internazionale</t>
+        </is>
+      </c>
+      <c r="D301" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E301" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="F301" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="G301" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="H301" t="inlineStr"/>
+      <c r="I301" t="inlineStr"/>
+      <c r="J301" t="inlineStr"/>
+      <c r="K301" t="n">
+        <v>2.39</v>
+      </c>
+      <c r="L301" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="M301" t="n">
+        <v>1.92</v>
+      </c>
+      <c r="N301" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="O301" t="n">
+        <v>1.16</v>
+      </c>
+      <c r="P301" t="inlineStr"/>
+      <c r="Q301" t="inlineStr"/>
+    </row>
+    <row r="302">
+      <c r="A302" s="2" t="n">
+        <v>45800.86458333334</v>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Napoli</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>Cagliari</t>
+        </is>
+      </c>
+      <c r="D302" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E302" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="F302" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="G302" t="n">
+        <v>14</v>
+      </c>
+      <c r="H302" t="inlineStr"/>
+      <c r="I302" t="inlineStr"/>
+      <c r="J302" t="inlineStr"/>
+      <c r="K302" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="L302" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M302" t="n">
+        <v>1.03</v>
+      </c>
+      <c r="N302" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="O302" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="P302" t="inlineStr"/>
+      <c r="Q302" t="inlineStr"/>
+    </row>
+    <row r="303">
+      <c r="A303" s="2" t="n">
+        <v>45801.67708333334</v>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Real Madrid</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="D303" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E303" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="F303" t="n">
+        <v>4.95</v>
+      </c>
+      <c r="G303" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H303" t="inlineStr"/>
+      <c r="I303" t="inlineStr"/>
+      <c r="J303" t="inlineStr"/>
+      <c r="K303" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="L303" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="M303" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N303" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="O303" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="P303" t="inlineStr"/>
+      <c r="Q303" t="inlineStr"/>
+    </row>
+    <row r="304">
+      <c r="A304" s="2" t="n">
+        <v>45801.75</v>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>Genoa</t>
+        </is>
+      </c>
+      <c r="D304" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E304" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="F304" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="G304" t="n">
+        <v>6</v>
+      </c>
+      <c r="H304" t="inlineStr"/>
+      <c r="I304" t="inlineStr"/>
+      <c r="J304" t="inlineStr"/>
+      <c r="K304" t="n">
+        <v>2.26</v>
+      </c>
+      <c r="L304" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="M304" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="N304" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="O304" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="P304" t="inlineStr"/>
+      <c r="Q304" t="inlineStr"/>
+    </row>
+    <row r="305">
+      <c r="A305" s="2" t="n">
+        <v>45801.75</v>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>Monza</t>
+        </is>
+      </c>
+      <c r="D305" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E305" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="F305" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="G305" t="n">
+        <v>11</v>
+      </c>
+      <c r="H305" t="inlineStr"/>
+      <c r="I305" t="inlineStr"/>
+      <c r="J305" t="inlineStr"/>
+      <c r="K305" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="L305" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="M305" t="n">
+        <v>1.05</v>
+      </c>
+      <c r="N305" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="O305" t="n">
+        <v>2.97</v>
+      </c>
+      <c r="P305" t="inlineStr"/>
+      <c r="Q305" t="inlineStr"/>
+    </row>
+    <row r="306">
+      <c r="A306" s="2" t="n">
+        <v>45801.77083333334</v>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Espanyol</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>Las Palmas</t>
+        </is>
+      </c>
+      <c r="D306" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E306" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="F306" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="G306" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="H306" t="inlineStr"/>
+      <c r="I306" t="inlineStr"/>
+      <c r="J306" t="inlineStr"/>
+      <c r="K306" t="n">
+        <v>1.93</v>
+      </c>
+      <c r="L306" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="M306" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="N306" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="O306" t="n">
+        <v>2.35</v>
+      </c>
+      <c r="P306" t="inlineStr"/>
+      <c r="Q306" t="inlineStr"/>
+    </row>
+    <row r="307">
+      <c r="A307" s="2" t="n">
+        <v>45801.77083333334</v>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Leganes</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>Valladolid</t>
+        </is>
+      </c>
+      <c r="D307" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E307" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="F307" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="G307" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="H307" t="inlineStr"/>
+      <c r="I307" t="inlineStr"/>
+      <c r="J307" t="inlineStr"/>
+      <c r="K307" t="n">
+        <v>2.11</v>
+      </c>
+      <c r="L307" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="M307" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="N307" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O307" t="n">
+        <v>2.61</v>
+      </c>
+      <c r="P307" t="inlineStr"/>
+      <c r="Q307" t="inlineStr"/>
+    </row>
+    <row r="308">
+      <c r="A308" s="2" t="n">
+        <v>45801.875</v>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Getafe</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>Celta Vigo</t>
+        </is>
+      </c>
+      <c r="D308" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E308" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="F308" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="G308" t="n">
+        <v>1.68</v>
+      </c>
+      <c r="H308" t="inlineStr"/>
+      <c r="I308" t="inlineStr"/>
+      <c r="J308" t="inlineStr"/>
+      <c r="K308" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="L308" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="M308" t="n">
+        <v>1.73</v>
+      </c>
+      <c r="N308" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="O308" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="P308" t="inlineStr"/>
+      <c r="Q308" t="inlineStr"/>
+    </row>
+    <row r="309">
+      <c r="A309" s="2" t="n">
+        <v>45801.875</v>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Alavés</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>Osasuna</t>
+        </is>
+      </c>
+      <c r="D309" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E309" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="F309" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="G309" t="n">
+        <v>1.82</v>
+      </c>
+      <c r="H309" t="inlineStr"/>
+      <c r="I309" t="inlineStr"/>
+      <c r="J309" t="inlineStr"/>
+      <c r="K309" t="n">
+        <v>1.58</v>
+      </c>
+      <c r="L309" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="M309" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="N309" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="O309" t="n">
+        <v>1.22</v>
+      </c>
+      <c r="P309" t="inlineStr"/>
+      <c r="Q309" t="inlineStr"/>
+    </row>
+    <row r="310">
+      <c r="A310" s="2" t="n">
+        <v>45801.875</v>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Rayo Vallecano</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>Mallorca</t>
+        </is>
+      </c>
+      <c r="D310" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E310" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="F310" t="n">
+        <v>3.95</v>
+      </c>
+      <c r="G310" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="H310" t="inlineStr"/>
+      <c r="I310" t="inlineStr"/>
+      <c r="J310" t="inlineStr"/>
+      <c r="K310" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="L310" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="M310" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N310" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O310" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="P310" t="inlineStr"/>
+      <c r="Q310" t="inlineStr"/>
+    </row>
+    <row r="311">
+      <c r="A311" s="2" t="n">
+        <v>45802.58333333334</v>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Girona</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>Atl. Madrid</t>
+        </is>
+      </c>
+      <c r="D311" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E311" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="F311" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="G311" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="H311" t="inlineStr"/>
+      <c r="I311" t="inlineStr"/>
+      <c r="J311" t="inlineStr"/>
+      <c r="K311" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="L311" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="M311" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="N311" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="O311" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="P311" t="inlineStr"/>
+      <c r="Q311" t="inlineStr"/>
+    </row>
+    <row r="312">
+      <c r="A312" s="2" t="n">
+        <v>45802.67708333334</v>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Villarreal</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="D312" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E312" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="F312" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="G312" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="H312" t="inlineStr"/>
+      <c r="I312" t="inlineStr"/>
+      <c r="J312" t="inlineStr"/>
+      <c r="K312" t="n">
+        <v>2.38</v>
+      </c>
+      <c r="L312" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="M312" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="N312" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="O312" t="n">
+        <v>2.07</v>
+      </c>
+      <c r="P312" t="inlineStr"/>
+      <c r="Q312" t="inlineStr"/>
+    </row>
+    <row r="313">
+      <c r="A313" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Manchester Utd.</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>Aston Villa</t>
+        </is>
+      </c>
+      <c r="D313" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E313" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="F313" t="n">
+        <v>4</v>
+      </c>
+      <c r="G313" t="n">
+        <v>1.64</v>
+      </c>
+      <c r="H313" t="inlineStr"/>
+      <c r="I313" t="inlineStr"/>
+      <c r="J313" t="inlineStr"/>
+      <c r="K313" t="n">
+        <v>2.44</v>
+      </c>
+      <c r="L313" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="M313" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="N313" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="O313" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="P313" t="inlineStr"/>
+      <c r="Q313" t="inlineStr"/>
+    </row>
+    <row r="314">
+      <c r="A314" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Wolverhampton</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>Brentford</t>
+        </is>
+      </c>
+      <c r="D314" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E314" t="n">
+        <v>2.78</v>
+      </c>
+      <c r="F314" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G314" t="n">
+        <v>2.08</v>
+      </c>
+      <c r="H314" t="inlineStr"/>
+      <c r="I314" t="inlineStr"/>
+      <c r="J314" t="inlineStr"/>
+      <c r="K314" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="L314" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M314" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="N314" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="O314" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="P314" t="inlineStr"/>
+      <c r="Q314" t="inlineStr"/>
+    </row>
+    <row r="315">
+      <c r="A315" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Ipswich</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>West Ham</t>
+        </is>
+      </c>
+      <c r="D315" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E315" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="F315" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G315" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="H315" t="inlineStr"/>
+      <c r="I315" t="inlineStr"/>
+      <c r="J315" t="inlineStr"/>
+      <c r="K315" t="n">
+        <v>2.47</v>
+      </c>
+      <c r="L315" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="M315" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="N315" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="O315" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="P315" t="inlineStr"/>
+      <c r="Q315" t="inlineStr"/>
+    </row>
+    <row r="316">
+      <c r="A316" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Newcastle</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>Everton</t>
+        </is>
+      </c>
+      <c r="D316" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E316" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F316" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="G316" t="n">
+        <v>8</v>
+      </c>
+      <c r="H316" t="inlineStr"/>
+      <c r="I316" t="inlineStr"/>
+      <c r="J316" t="inlineStr"/>
+      <c r="K316" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="L316" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M316" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="N316" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O316" t="n">
+        <v>2.51</v>
+      </c>
+      <c r="P316" t="inlineStr"/>
+      <c r="Q316" t="inlineStr"/>
+    </row>
+    <row r="317">
+      <c r="A317" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Southampton</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="D317" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E317" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="F317" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="G317" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="H317" t="inlineStr"/>
+      <c r="I317" t="inlineStr"/>
+      <c r="J317" t="inlineStr"/>
+      <c r="K317" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="L317" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M317" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="N317" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="O317" t="n">
+        <v>1.08</v>
+      </c>
+      <c r="P317" t="inlineStr"/>
+      <c r="Q317" t="inlineStr"/>
+    </row>
+    <row r="318">
+      <c r="A318" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>Brighton</t>
+        </is>
+      </c>
+      <c r="D318" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E318" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="F318" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="G318" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="H318" t="inlineStr"/>
+      <c r="I318" t="inlineStr"/>
+      <c r="J318" t="inlineStr"/>
+      <c r="K318" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="L318" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="M318" t="n">
+        <v>1.63</v>
+      </c>
+      <c r="N318" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O318" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="P318" t="inlineStr"/>
+      <c r="Q318" t="inlineStr"/>
+    </row>
+    <row r="319">
+      <c r="A319" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Liverpool</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>Crystal Palace</t>
+        </is>
+      </c>
+      <c r="D319" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E319" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="F319" t="n">
+        <v>5</v>
+      </c>
+      <c r="G319" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="H319" t="inlineStr"/>
+      <c r="I319" t="inlineStr"/>
+      <c r="J319" t="inlineStr"/>
+      <c r="K319" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="L319" t="n">
+        <v>1.45</v>
+      </c>
+      <c r="M319" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="N319" t="n">
+        <v>1.14</v>
+      </c>
+      <c r="O319" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="P319" t="inlineStr"/>
+      <c r="Q319" t="inlineStr"/>
+    </row>
+    <row r="320">
+      <c r="A320" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Fulham</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>Manchester City</t>
+        </is>
+      </c>
+      <c r="D320" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E320" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="F320" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="G320" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="H320" t="inlineStr"/>
+      <c r="I320" t="inlineStr"/>
+      <c r="J320" t="inlineStr"/>
+      <c r="K320" t="n">
+        <v>2.56</v>
+      </c>
+      <c r="L320" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M320" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="N320" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O320" t="n">
+        <v>1.17</v>
+      </c>
+      <c r="P320" t="inlineStr"/>
+      <c r="Q320" t="inlineStr"/>
+    </row>
+    <row r="321">
+      <c r="A321" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Bournemouth</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>Leicester</t>
+        </is>
+      </c>
+      <c r="D321" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E321" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="F321" t="n">
+        <v>5.25</v>
+      </c>
+      <c r="G321" t="n">
+        <v>8</v>
+      </c>
+      <c r="H321" t="inlineStr"/>
+      <c r="I321" t="inlineStr"/>
+      <c r="J321" t="inlineStr"/>
+      <c r="K321" t="n">
+        <v>2.59</v>
+      </c>
+      <c r="L321" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="M321" t="n">
+        <v>1.07</v>
+      </c>
+      <c r="N321" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="O321" t="n">
+        <v>2.52</v>
+      </c>
+      <c r="P321" t="inlineStr"/>
+      <c r="Q321" t="inlineStr"/>
+    </row>
+    <row r="322">
+      <c r="A322" s="2" t="n">
+        <v>45802.70833333334</v>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Nottingham</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="D322" t="inlineStr">
+        <is>
+          <t>ENG1</t>
+        </is>
+      </c>
+      <c r="E322" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F322" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="G322" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H322" t="inlineStr"/>
+      <c r="I322" t="inlineStr"/>
+      <c r="J322" t="inlineStr"/>
+      <c r="K322" t="n">
+        <v>2.24</v>
+      </c>
+      <c r="L322" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="M322" t="n">
+        <v>1.57</v>
+      </c>
+      <c r="N322" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="O322" t="n">
+        <v>1.28</v>
+      </c>
+      <c r="P322" t="inlineStr"/>
+      <c r="Q322" t="inlineStr"/>
+    </row>
+    <row r="323">
+      <c r="A323" s="2" t="n">
+        <v>45802.86458333334</v>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Udinese</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>Fiorentina</t>
+        </is>
+      </c>
+      <c r="D323" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E323" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="F323" t="n">
+        <v>3.55</v>
+      </c>
+      <c r="G323" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="H323" t="inlineStr"/>
+      <c r="I323" t="inlineStr"/>
+      <c r="J323" t="inlineStr"/>
+      <c r="K323" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="L323" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="M323" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="N323" t="n">
+        <v>1.25</v>
+      </c>
+      <c r="O323" t="n">
+        <v>1.23</v>
+      </c>
+      <c r="P323" t="inlineStr"/>
+      <c r="Q323" t="inlineStr"/>
+    </row>
+    <row r="324">
+      <c r="A324" s="2" t="n">
+        <v>45802.86458333334</v>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Lazio</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>Lecce</t>
+        </is>
+      </c>
+      <c r="D324" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E324" t="n">
+        <v>1.33</v>
+      </c>
+      <c r="F324" t="n">
+        <v>4.65</v>
+      </c>
+      <c r="G324" t="n">
+        <v>7</v>
+      </c>
+      <c r="H324" t="inlineStr"/>
+      <c r="I324" t="inlineStr"/>
+      <c r="J324" t="inlineStr"/>
+      <c r="K324" t="n">
+        <v>2.22</v>
+      </c>
+      <c r="L324" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="M324" t="n">
+        <v>1.09</v>
+      </c>
+      <c r="N324" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="O324" t="n">
+        <v>2.28</v>
+      </c>
+      <c r="P324" t="inlineStr"/>
+      <c r="Q324" t="inlineStr"/>
+    </row>
+    <row r="325">
+      <c r="A325" s="2" t="n">
+        <v>45802.86458333334</v>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>Parma</t>
+        </is>
+      </c>
+      <c r="D325" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E325" t="n">
+        <v>1.36</v>
+      </c>
+      <c r="F325" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="G325" t="n">
+        <v>6</v>
+      </c>
+      <c r="H325" t="inlineStr"/>
+      <c r="I325" t="inlineStr"/>
+      <c r="J325" t="inlineStr"/>
+      <c r="K325" t="n">
+        <v>2.75</v>
+      </c>
+      <c r="L325" t="n">
+        <v>1.44</v>
+      </c>
+      <c r="M325" t="n">
+        <v>1.12</v>
+      </c>
+      <c r="N325" t="n">
+        <v>1.15</v>
+      </c>
+      <c r="O325" t="n">
+        <v>2.19</v>
+      </c>
+      <c r="P325" t="inlineStr"/>
+      <c r="Q325" t="inlineStr"/>
+    </row>
+    <row r="326">
+      <c r="A326" s="2" t="n">
+        <v>45802.86458333334</v>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Venezia</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="D326" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E326" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F326" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G326" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="H326" t="inlineStr"/>
+      <c r="I326" t="inlineStr"/>
+      <c r="J326" t="inlineStr"/>
+      <c r="K326" t="n">
+        <v>1.97</v>
+      </c>
+      <c r="L326" t="n">
+        <v>1.84</v>
+      </c>
+      <c r="M326" t="n">
+        <v>2</v>
+      </c>
+      <c r="N326" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="O326" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="P326" t="inlineStr"/>
+      <c r="Q326" t="inlineStr"/>
+    </row>
+    <row r="327">
+      <c r="A327" s="2" t="n">
+        <v>45802.86458333334</v>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>Roma</t>
+        </is>
+      </c>
+      <c r="D327" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E327" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="F327" t="n">
+        <v>4</v>
+      </c>
+      <c r="G327" t="n">
+        <v>1.47</v>
+      </c>
+      <c r="H327" t="inlineStr"/>
+      <c r="I327" t="inlineStr"/>
+      <c r="J327" t="inlineStr"/>
+      <c r="K327" t="n">
+        <v>1.89</v>
+      </c>
+      <c r="L327" t="n">
+        <v>1.91</v>
+      </c>
+      <c r="M327" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="N327" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="O327" t="n">
+        <v>1.13</v>
+      </c>
+      <c r="P327" t="inlineStr"/>
+      <c r="Q327" t="inlineStr"/>
+    </row>
+    <row r="328">
+      <c r="A328" s="2" t="n">
+        <v>45802.86458333334</v>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Empoli</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>Hellas Verona</t>
+        </is>
+      </c>
+      <c r="D328" t="inlineStr">
+        <is>
+          <t>ITA1</t>
+        </is>
+      </c>
+      <c r="E328" t="n">
+        <v>1.77</v>
+      </c>
+      <c r="F328" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="G328" t="n">
+        <v>4.05</v>
+      </c>
+      <c r="H328" t="inlineStr"/>
+      <c r="I328" t="inlineStr"/>
+      <c r="J328" t="inlineStr"/>
+      <c r="K328" t="n">
+        <v>1.67</v>
+      </c>
+      <c r="L328" t="n">
+        <v>2.21</v>
+      </c>
+      <c r="M328" t="n">
+        <v>1.21</v>
+      </c>
+      <c r="N328" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="O328" t="n">
+        <v>1.65</v>
+      </c>
+      <c r="P328" t="inlineStr"/>
+      <c r="Q328" t="inlineStr"/>
+    </row>
+    <row r="329">
+      <c r="A329" s="2" t="n">
+        <v>45802.875</v>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Ath. Bilbao</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="D329" t="inlineStr">
+        <is>
+          <t>ESP1</t>
+        </is>
+      </c>
+      <c r="E329" t="n">
+        <v>3.05</v>
+      </c>
+      <c r="F329" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="G329" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="H329" t="inlineStr"/>
+      <c r="I329" t="inlineStr"/>
+      <c r="J329" t="inlineStr"/>
+      <c r="K329" t="n">
+        <v>2.36</v>
+      </c>
+      <c r="L329" t="n">
+        <v>1.46</v>
+      </c>
+      <c r="M329" t="n">
+        <v>1.53</v>
+      </c>
+      <c r="N329" t="n">
+        <v>1.24</v>
+      </c>
+      <c r="O329" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="P329" t="inlineStr"/>
+      <c r="Q329" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>